<commit_message>
update full function v1
</commit_message>
<xml_diff>
--- a/registry-total-backend/src/main/resources/Web_Data_Final.xlsx
+++ b/registry-total-backend/src/main/resources/Web_Data_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UET\Web\registry-total\registry-total-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1554A4-1C99-43DF-BDC8-D6DB4E0BC572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A0909-2868-4307-B4A9-CA7FBA562BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách xe" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="243">
   <si>
     <t>STT</t>
   </si>
@@ -544,12 +544,6 @@
     <t>Hạn hiệu lực đăng kiểm</t>
   </si>
   <si>
-    <t>Trung tâm đăng kiểm</t>
-  </si>
-  <si>
-    <t>2903S</t>
-  </si>
-  <si>
     <t>1502S</t>
   </si>
   <si>
@@ -565,16 +559,10 @@
     <t>1501V</t>
   </si>
   <si>
-    <t>2902V</t>
-  </si>
-  <si>
     <t>3701S</t>
   </si>
   <si>
     <t>3801D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901V </t>
   </si>
   <si>
     <t>Username</t>
@@ -1331,10 +1319,10 @@
         <v>20</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>21</v>
@@ -1390,10 +1378,10 @@
         <v>28</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>21</v>
@@ -31049,10 +31037,10 @@
         <v>117</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>118</v>
@@ -61427,9 +61415,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -61437,7 +61427,7 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -61453,11 +61443,8 @@
       <c r="E1" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="31">
         <v>1</v>
       </c>
@@ -61473,11 +61460,8 @@
       <c r="E2" s="32">
         <v>45281</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>2</v>
       </c>
@@ -61493,11 +61477,8 @@
       <c r="E3" s="32">
         <v>45391</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="31">
         <v>3</v>
       </c>
@@ -61513,11 +61494,8 @@
       <c r="E4" s="32">
         <v>45575</v>
       </c>
-      <c r="F4" s="31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
         <v>4</v>
       </c>
@@ -61533,11 +61511,8 @@
       <c r="E5" s="32">
         <v>45154</v>
       </c>
-      <c r="F5" s="31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="31">
         <v>5</v>
       </c>
@@ -61553,11 +61528,8 @@
       <c r="E6" s="32">
         <v>45605</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="31">
         <v>6</v>
       </c>
@@ -61573,11 +61545,8 @@
       <c r="E7" s="32">
         <v>45098</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="31">
         <v>7</v>
       </c>
@@ -61593,11 +61562,8 @@
       <c r="E8" s="32">
         <v>45333</v>
       </c>
-      <c r="F8" s="31" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="31">
         <v>8</v>
       </c>
@@ -61613,11 +61579,8 @@
       <c r="E9" s="32">
         <v>45329</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="31">
         <v>9</v>
       </c>
@@ -61633,11 +61596,8 @@
       <c r="E10" s="32">
         <v>45180</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="31">
         <v>10</v>
       </c>
@@ -61653,25 +61613,20 @@
       <c r="E11" s="32">
         <v>45449</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="31"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -61685,7 +61640,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -61697,24 +61652,24 @@
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -61722,16 +61677,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>16</v>
@@ -61742,16 +61697,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>16</v>
@@ -61762,16 +61717,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>16</v>
@@ -61782,242 +61737,242 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>12</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -62025,7 +61980,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -62033,7 +61988,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -62041,7 +61996,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -62049,7 +62004,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -62057,7 +62012,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -62065,7 +62020,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -62073,7 +62028,7 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -62081,7 +62036,7 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -62089,7 +62044,7 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -62097,7 +62052,7 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -62105,7 +62060,7 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -62113,7 +62068,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -62121,7 +62076,7 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -62129,7 +62084,7 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -62137,7 +62092,7 @@
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>

</xml_diff>